<commit_message>
Adds merged, documented version of the Code
</commit_message>
<xml_diff>
--- a/new/output1/asquant_group1_Vs_group2.xlsx
+++ b/new/output1/asquant_group1_Vs_group2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
   <si>
     <t>chrom</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>chr10:ZUFSP:33935088-33935257</t>
+  </si>
+  <si>
+    <t>NCOA7</t>
+  </si>
+  <si>
+    <t>chr10:NCOA7:30691755-30691787</t>
   </si>
 </sst>
 </file>
@@ -781,7 +787,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -823,6 +829,44 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>30691755</v>
+      </c>
+      <c r="D2">
+        <v>30691787</v>
+      </c>
+      <c r="E2">
+        <v>0.8698350074869731</v>
+      </c>
+      <c r="F2">
+        <v>0.026160299348494</v>
+      </c>
+      <c r="G2">
+        <v>0.026160299348494</v>
+      </c>
+      <c r="H2">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="I2">
+        <v>95.53465184700885</v>
+      </c>
+      <c r="J2">
+        <v>102.7272727272727</v>
+      </c>
+      <c r="K2">
+        <v>123.4163125204315</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>